<commit_message>
added methods to get list of individual sheets as well as the number of visible sheets
</commit_message>
<xml_diff>
--- a/booneexcelsub.xlsx
+++ b/booneexcelsub.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\newproj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fdumont\Downloads\Statistical-Performance-Measures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2494D5-D7EA-4741-91F9-17452AFC91B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C122D66-383C-43E9-A228-F81E235BD02C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="3195" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3574B3EA-4937-494C-82DC-A3A1D49C4B09}"/>
+    <workbookView xWindow="26385" yWindow="-4560" windowWidth="15375" windowHeight="7875" xr2:uid="{3574B3EA-4937-494C-82DC-A3A1D49C4B09}"/>
   </bookViews>
   <sheets>
     <sheet name="6-8-11" sheetId="5" r:id="rId1"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59A842A-9BEA-4E91-A85D-9F02313152EC}">
   <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="J142" sqref="J1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11119,7 +11119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949635F4-0BD7-4C3F-BE0B-9783119533F8}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F182" sqref="F182"/>
     </sheetView>
   </sheetViews>

</xml_diff>